<commit_message>
some refactoring just before 11 am break
</commit_message>
<xml_diff>
--- a/new_colleagues.xlsx
+++ b/new_colleagues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/69beb3b4f394b148/BeCode/challenger-openspace-classifier/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{328D644F-2300-4EA8-A37E-EE9F3C7BAB49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D518D6A-766B-470C-A536-228416B7C2CE}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{328D644F-2300-4EA8-A37E-EE9F3C7BAB49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97AD6264-CF97-488B-B37E-1A6348D899B7}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -636,6 +636,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -937,8 +941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>